<commit_message>
Made U8 component (clock buffer) DNP.
</commit_message>
<xml_diff>
--- a/hardware/RFWBBoard/RFWBBoard_BOM.xlsx
+++ b/hardware/RFWBBoard/RFWBBoard_BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="152">
   <si>
     <t>Item #</t>
   </si>
@@ -485,7 +485,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -550,6 +550,14 @@
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -658,14 +666,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -789,11 +798,28 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Excel_BuiltIn_Calculation 1" xfId="3"/>
     <cellStyle name="Excel_BuiltIn_Explanatory Text 1" xfId="2"/>
     <cellStyle name="Excel_BuiltIn_Heading 3 1" xfId="1"/>
+    <cellStyle name="Explanatory Text" xfId="5" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
@@ -1185,7 +1211,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,37 +2060,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+    <row r="25" spans="1:12" s="56" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="51">
         <v>22</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7" t="s">
+      <c r="C25" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="52" t="s">
         <v>138</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I25" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="J25" s="8">
+      <c r="J25" s="54">
         <v>1</v>
       </c>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9">
+      <c r="K25" s="55"/>
+      <c r="L25" s="55">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
- BOM updated - pull down resistor for SHDN - Names arranged
</commit_message>
<xml_diff>
--- a/hardware/RFWBBoard/RFWBBoard_BOM.xlsx
+++ b/hardware/RFWBBoard/RFWBBoard_BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="120" windowWidth="16380" windowHeight="8070" tabRatio="353"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="183">
   <si>
     <t>Item #</t>
   </si>
@@ -58,9 +58,6 @@
     <t>MEZZANINE 1MM BTB RECPT 84CKT</t>
   </si>
   <si>
-    <t>R41, R47, R48, R51, R57, R58</t>
-  </si>
-  <si>
     <t>0402 (1005 Metric)</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>RES 49.9 OHM .125W 1% 0402 SMD</t>
   </si>
   <si>
-    <t>R42, R52, R65, R66, R75, R76</t>
-  </si>
-  <si>
     <t xml:space="preserve">Panasonic - ECG </t>
   </si>
   <si>
@@ -91,18 +85,6 @@
     <t>RES 24.9 OHM 1/10W 1% 0402 SMD</t>
   </si>
   <si>
-    <t>R43, R44, R45, R46, R53, R54, R55, R56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-2RKF3480X </t>
-  </si>
-  <si>
-    <t xml:space="preserve">P348LCT-ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES 348 OHM 1/10W 1% 0402 SMD </t>
-  </si>
-  <si>
     <t>R451, R452, R671, R672</t>
   </si>
   <si>
@@ -152,9 +134,6 @@
   </si>
   <si>
     <t xml:space="preserve">IC AMP DIFF LDIST LP 70MA 8MSOP </t>
-  </si>
-  <si>
-    <t>X1, X2, X4, X5, X6, X7</t>
   </si>
   <si>
     <t>IC1</t>
@@ -376,27 +355,12 @@
     <t>Total</t>
   </si>
   <si>
-    <t>C114, C123, C126, C129</t>
-  </si>
-  <si>
-    <t>C115, C117, C42, C45, C52, C62, C67, C72, C102, C124, C127, C130</t>
-  </si>
-  <si>
     <t>C109, C110, C111, C112, C113, C43, C53, C63, C73</t>
   </si>
   <si>
-    <t>C121, C122</t>
-  </si>
-  <si>
     <t>DNP</t>
   </si>
   <si>
-    <t>C104, R3, R4, RWP0, RWP1, RA20, RA21, RA10, RA11, RA00, RA01</t>
-  </si>
-  <si>
-    <t>C103, C106, C107, C108, C116, C120, C64, C74, C125, C128, C131</t>
-  </si>
-  <si>
     <t>C41, C51, C61, C71, C101</t>
   </si>
   <si>
@@ -427,39 +391,6 @@
     <t xml:space="preserve"> CONNECTOR FEMALE SMD</t>
   </si>
   <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>X3</t>
-  </si>
-  <si>
-    <t>8-SOIC</t>
-  </si>
-  <si>
-    <t>Integrated Device Technology Inc</t>
-  </si>
-  <si>
-    <t>ICS83021AMILF</t>
-  </si>
-  <si>
-    <t>800-1100-5-ND</t>
-  </si>
-  <si>
-    <t>IC FANOUT BUFFER SGL I/O 8-SOIC</t>
-  </si>
-  <si>
-    <t>ICS85320AMILF</t>
-  </si>
-  <si>
-    <t>800-1168-5-ND</t>
-  </si>
-  <si>
-    <t>IC TRANSLATOR LVPECL 8-SOIC</t>
-  </si>
-  <si>
     <t>4-SMD, No Lead (DFN, LCC)</t>
   </si>
   <si>
@@ -475,7 +406,169 @@
     <t>OSCILLATOR TCXO 20.0MHZ 3.3V SMD</t>
   </si>
   <si>
-    <t>Bill of Materials for 'Marmote - Wide Band RF Board (Rev A)'</t>
+    <t>Bill of Materials for 'Marmote - Wide Band RF Board (Rev B)'</t>
+  </si>
+  <si>
+    <t>C115, C117, C42, C45, C52, C62, C67, C72, C102, C124</t>
+  </si>
+  <si>
+    <t>R65, R66, R75, R76</t>
+  </si>
+  <si>
+    <t>R47, R48, R57, R58</t>
+  </si>
+  <si>
+    <t>R43, R44, R53, R54</t>
+  </si>
+  <si>
+    <t>R45, R46, R55, R56</t>
+  </si>
+  <si>
+    <t>1.58k</t>
+  </si>
+  <si>
+    <t>1.3k</t>
+  </si>
+  <si>
+    <t>C103, C106, C107, C108, C116, C120, C64, C74, C125</t>
+  </si>
+  <si>
+    <t>C121</t>
+  </si>
+  <si>
+    <t>C126</t>
+  </si>
+  <si>
+    <t>C114, C123</t>
+  </si>
+  <si>
+    <t>J2, J3, J4, J5, J6, J7, J8</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>R41, R42, R51, R52</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>C127</t>
+  </si>
+  <si>
+    <t>C128</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>RWP0, RA20, RA10,  RA00, R6</t>
+  </si>
+  <si>
+    <t>C104, RWP1, RA21, RA11, RA01, R5, R4</t>
+  </si>
+  <si>
+    <t>ERJ-2GE0R00X</t>
+  </si>
+  <si>
+    <t>P0.0JDKR-ND</t>
+  </si>
+  <si>
+    <t>RES 0.0 OHM 1/10W 0402 SMD</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1581X</t>
+  </si>
+  <si>
+    <t>P1.58KLDKR-ND</t>
+  </si>
+  <si>
+    <t>RES 1.58K OHM 1/10W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1301X</t>
+  </si>
+  <si>
+    <t>P1.30KLDKR-ND</t>
+  </si>
+  <si>
+    <t>RES 1.30K OHM 1/10W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>CRCW040210K0FKEDHP</t>
+  </si>
+  <si>
+    <t>541-10.0KYCT-ND</t>
+  </si>
+  <si>
+    <t>RES 10.0K OHM .125W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>GRM1555C1H180JA01D</t>
+  </si>
+  <si>
+    <t>81-GRM1555C1H180JA1D</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0402 18pF 50volts C0G 5%</t>
+  </si>
+  <si>
+    <t>GRM1555C1H330JA01D</t>
+  </si>
+  <si>
+    <t>81-GRM1555C1H330JA1D</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0402 33pF 50volts C0G 5%</t>
+  </si>
+  <si>
+    <t>Kyocera</t>
+  </si>
+  <si>
+    <t>478-4817-1-ND</t>
+  </si>
+  <si>
+    <t>CX101F-040.000-H0445</t>
+  </si>
+  <si>
+    <t>CRYSTAL 40.000MHZ 12PF SMD</t>
+  </si>
+  <si>
+    <t>DNP (1000pF)</t>
+  </si>
+  <si>
+    <t>DNP (18pF)</t>
+  </si>
+  <si>
+    <t>DNP (33pF)</t>
+  </si>
+  <si>
+    <t>R7, R8, R9</t>
+  </si>
+  <si>
+    <t>30k</t>
+  </si>
+  <si>
+    <t>1206 (3216 Metric)</t>
+  </si>
+  <si>
+    <t>P0.0ECT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-8GEY0R00V</t>
+  </si>
+  <si>
+    <t>RES 0.0 OHM 1/4W 1206 SMD</t>
+  </si>
+  <si>
+    <t>ERJ-2GEJ303X</t>
+  </si>
+  <si>
+    <t>P30KJCT-ND</t>
+  </si>
+  <si>
+    <t>RES 30K OHM 1/10W 5% 0402 SMD</t>
   </si>
 </sst>
 </file>
@@ -552,12 +645,10 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -666,15 +757,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -798,28 +888,40 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="Excel_BuiltIn_Calculation 1" xfId="3"/>
     <cellStyle name="Excel_BuiltIn_Explanatory Text 1" xfId="2"/>
     <cellStyle name="Excel_BuiltIn_Heading 3 1" xfId="1"/>
-    <cellStyle name="Explanatory Text" xfId="5" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
@@ -1208,16 +1310,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="60" customWidth="1"/>
-    <col min="3" max="3" width="16" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="1" customWidth="1"/>
@@ -1231,7 +1334,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -1274,19 +1377,19 @@
         <v>4</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="G3" s="41" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="I3" s="41" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="41" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="K3" s="41" t="s">
         <v>6</v>
@@ -1330,1083 +1433,1366 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
+        <f>A4+1</f>
         <v>2</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="7">
-        <v>24.9</v>
+        <v>113</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>15</v>
+        <v>114</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>24</v>
+        <v>118</v>
       </c>
       <c r="J5" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9">
-        <f t="shared" ref="L5" si="0">J5*K5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="L5:L37" si="0">J5*K5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
+        <f t="shared" ref="A6:A32" si="1">A5+1</f>
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7">
-        <v>49.9</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="J6" s="8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9">
-        <f t="shared" ref="L6:L29" si="1">J6*K6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="6">
-        <v>348</v>
+        <v>130</v>
+      </c>
+      <c r="C7" s="7">
+        <v>24.9</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J7" s="8">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9">
-        <f t="shared" ref="L7:L10" si="2">J7*K7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="6">
-        <v>750</v>
+        <v>131</v>
+      </c>
+      <c r="C8" s="7">
+        <v>49.9</v>
       </c>
       <c r="D8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="F8" s="6" t="s">
-        <v>95</v>
+        <v>16</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="J8" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>99</v>
+        <v>87</v>
+      </c>
+      <c r="C9" s="6">
+        <v>750</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="J9" s="8">
         <v>1</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="J10" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>30</v>
+        <v>102</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="J11" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>35</v>
+      <c r="B12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="15">
-        <v>8</v>
+        <v>26</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="8">
+        <v>4</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>81</v>
+      <c r="B13" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>51</v>
+        <v>30</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="J13" s="8">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="15">
+        <v>8</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9">
-        <f t="shared" ref="L13:L23" si="3">J13*K13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="J14" s="8">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>90</v>
+        <v>33</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="J15" s="8">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="I16" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="J16" s="8">
         <v>1</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="J17" s="8">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="J18" s="8">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>125</v>
+        <v>56</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>126</v>
+        <v>57</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>127</v>
+        <v>49</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>11</v>
+        <v>59</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>130</v>
+        <v>60</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="J19" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>63</v>
+        <v>139</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>66</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="7" t="s">
         <v>68</v>
       </c>
       <c r="J20" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>55</v>
+        <v>96</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="J21" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7" t="s">
-        <v>104</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
       <c r="E22" s="6" t="s">
-        <v>105</v>
+        <v>49</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>108</v>
+        <v>52</v>
       </c>
       <c r="J22" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="E23" s="6" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="J23" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="C24" s="6"/>
-      <c r="D24" s="11" t="s">
-        <v>41</v>
-      </c>
+      <c r="D24" s="7"/>
       <c r="E24" s="6" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>43</v>
+        <v>120</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>44</v>
+        <v>121</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="J24" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K24" s="9"/>
       <c r="L24" s="9">
-        <f t="shared" ref="L24:L26" si="4">J24*K24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="56" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B25" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="C25" s="53" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" s="52" t="s">
-        <v>138</v>
-      </c>
-      <c r="E25" s="53" t="s">
-        <v>139</v>
-      </c>
-      <c r="F25" s="53" t="s">
-        <v>140</v>
-      </c>
-      <c r="G25" s="53" t="s">
+      <c r="B25" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="I25" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="J25" s="54">
+      <c r="H25" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="J25" s="8">
         <v>1</v>
       </c>
-      <c r="K25" s="55"/>
-      <c r="L25" s="55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="9"/>
+      <c r="L25" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="7" t="s">
-        <v>138</v>
+        <v>41</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>143</v>
+        <v>43</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>144</v>
+        <v>45</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>145</v>
+        <v>46</v>
       </c>
       <c r="J26" s="8">
         <v>1</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="F27" s="6" t="s">
+      <c r="B27" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" s="55">
+        <v>0</v>
+      </c>
+      <c r="D27" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="51" t="s">
+        <v>150</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="J27" s="51">
+        <v>5</v>
+      </c>
+      <c r="K27" s="51"/>
+      <c r="L27" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="51"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="C28" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="G28" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H28" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="J28" s="53">
+        <v>4</v>
+      </c>
+      <c r="K28" s="54"/>
+      <c r="L28" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="51"/>
+    </row>
+    <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="I27" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="J27" s="8">
-        <v>6</v>
-      </c>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9">
-        <f t="shared" ref="L27:L28" si="5">J27*K27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>25</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7" t="s">
+      <c r="C29" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="J29" s="53">
+        <v>4</v>
+      </c>
+      <c r="K29" s="54"/>
+      <c r="L29" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="51"/>
+    </row>
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="J30" s="53">
+        <v>4</v>
+      </c>
+      <c r="K30" s="54"/>
+      <c r="L30" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="51"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" s="14">
+        <v>0</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="J31" s="53">
+        <v>3</v>
+      </c>
+      <c r="K31" s="54"/>
+      <c r="L31" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="51"/>
+    </row>
+    <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D32" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="J32" s="53">
+        <v>1</v>
+      </c>
+      <c r="K32" s="54"/>
+      <c r="L32" s="9">
+        <f>J32*K32</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="51"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="46">
+        <f>A32+1</f>
+        <v>30</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="45">
+        <v>7</v>
+      </c>
+      <c r="K33" s="47"/>
+      <c r="L33" s="9"/>
+    </row>
+    <row r="34" spans="1:12" s="61" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="46">
+        <f t="shared" ref="A34:A37" si="2">A33+1</f>
+        <v>31</v>
+      </c>
+      <c r="B34" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="G34" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="H34" s="57" t="s">
+        <v>85</v>
+      </c>
+      <c r="I34" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="J34" s="59">
+        <v>1</v>
+      </c>
+      <c r="K34" s="60"/>
+      <c r="L34" s="9"/>
+    </row>
+    <row r="35" spans="1:12" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="46">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="B35" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="57" t="s">
+        <v>172</v>
+      </c>
+      <c r="D35" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="56" t="s">
+        <v>161</v>
+      </c>
+      <c r="G35" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="H35" s="57" t="s">
+        <v>162</v>
+      </c>
+      <c r="I35" s="56" t="s">
+        <v>163</v>
+      </c>
+      <c r="J35" s="59">
+        <v>1</v>
+      </c>
+      <c r="K35" s="60"/>
+      <c r="L35" s="9"/>
+    </row>
+    <row r="36" spans="1:12" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="46">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="B36" s="56" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" s="57" t="s">
+        <v>173</v>
+      </c>
+      <c r="D36" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="G36" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="H36" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="I36" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="J36" s="59">
+        <v>1</v>
+      </c>
+      <c r="K36" s="60"/>
+      <c r="L36" s="9"/>
+    </row>
+    <row r="37" spans="1:12" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="46">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="B37" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G28" s="6" t="s">
+      <c r="C37" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" s="57" t="s">
+        <v>169</v>
+      </c>
+      <c r="G37" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="J28" s="8">
+      <c r="H37" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="I37" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="J37" s="59">
         <v>1</v>
       </c>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>26</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J29" s="8">
-        <v>1</v>
-      </c>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="46">
-        <v>27</v>
-      </c>
-      <c r="B30" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="C30" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="45">
-        <v>10</v>
-      </c>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47">
-        <f t="shared" ref="L30" si="6">I30*K30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="J31" s="48">
-        <f>SUM(J4:J30)</f>
+      <c r="K37" s="60"/>
+      <c r="L37" s="9"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="L31" s="3">
-        <f>SUM(L4:L30)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="17"/>
-    </row>
-    <row r="33" spans="2:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="18"/>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="20"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="23"/>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="17"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36"/>
-      <c r="L36"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="27"/>
-      <c r="J37"/>
-      <c r="L37"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="31"/>
-      <c r="J38"/>
-      <c r="L38"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="31"/>
-      <c r="J39"/>
-      <c r="L39"/>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="31"/>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="37"/>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="30"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="38"/>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="30"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
-      <c r="I43" s="38"/>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="39"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="38"/>
+      <c r="J38" s="48">
+        <f>SUM(J4:J37)</f>
+        <v>111</v>
+      </c>
+      <c r="L38" s="3">
+        <f>SUM(L4:L27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="17"/>
+    </row>
+    <row r="40" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="18"/>
+      <c r="L40" s="3"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="20"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="23"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="17"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43"/>
+      <c r="L43"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="27"/>
+      <c r="J44"/>
+      <c r="L44"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="31"/>
+      <c r="J45"/>
+      <c r="L45"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="28"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="31"/>
+      <c r="J46"/>
+      <c r="L46"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="31"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="37"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="30"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="38"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="30"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="38"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="39"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="38"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Modified the BOM file so that the 40 MHz crystal is populated (and is selected by default).
</commit_message>
<xml_diff>
--- a/hardware/RFWBBoard/RFWBBoard_BOM.xlsx
+++ b/hardware/RFWBBoard/RFWBBoard_BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="183">
   <si>
     <t>Item #</t>
   </si>
@@ -535,12 +535,6 @@
     <t>DNP (1000pF)</t>
   </si>
   <si>
-    <t>DNP (18pF)</t>
-  </si>
-  <si>
-    <t>DNP (33pF)</t>
-  </si>
-  <si>
     <t>R7, R8, R9</t>
   </si>
   <si>
@@ -569,6 +563,12 @@
   </si>
   <si>
     <t>Bill of Materials for 'Marmote - Wide Band RF Board Rev B (Joshua)'</t>
+  </si>
+  <si>
+    <t>18pF</t>
+  </si>
+  <si>
+    <t>33pF</t>
   </si>
 </sst>
 </file>
@@ -764,7 +764,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -873,9 +873,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -915,6 +912,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1314,11 +1317,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="46.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
@@ -1333,23 +1337,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="60" t="s">
-        <v>182</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
+      <c r="A1" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -1433,7 +1436,6 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <f>A4+1</f>
         <v>2</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -1465,13 +1467,12 @@
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9">
-        <f t="shared" ref="L5:L31" si="0">J5*K5</f>
+        <f t="shared" ref="L5:L30" si="0">J5*K5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <f t="shared" ref="A6:A32" si="1">A5+1</f>
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1509,7 +1510,6 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -1547,7 +1547,6 @@
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1585,7 +1584,6 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -1623,7 +1621,6 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -1661,7 +1658,6 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -1699,7 +1695,6 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -1737,7 +1732,6 @@
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B13" s="12" t="s">
@@ -1775,7 +1769,6 @@
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -1813,7 +1806,6 @@
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -1851,14 +1843,13 @@
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>14</v>
@@ -1867,16 +1858,16 @@
         <v>49</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>44</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J16" s="8">
         <v>1</v>
@@ -1889,14 +1880,13 @@
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>14</v>
@@ -1905,19 +1895,19 @@
         <v>49</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>44</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="J17" s="8">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9">
@@ -1927,35 +1917,34 @@
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>14</v>
+        <v>57</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>49</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>44</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="J18" s="8">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9">
@@ -1965,35 +1954,34 @@
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>56</v>
+        <v>138</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>49</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>44</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>61</v>
+        <v>67</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="J19" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9">
@@ -2003,35 +1991,32 @@
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>48</v>
+        <v>96</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="J20" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9">
@@ -2039,35 +2024,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7" t="s">
-        <v>97</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="6" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="J21" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9">
@@ -2075,33 +2057,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="E22" s="6" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="J22" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9">
@@ -2109,35 +2092,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="11" t="s">
-        <v>35</v>
-      </c>
+      <c r="D23" s="7"/>
       <c r="E23" s="6" t="s">
-        <v>36</v>
+        <v>119</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
       <c r="J23" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9">
@@ -2145,33 +2125,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
+      <c r="D24" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="E24" s="6" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="J24" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K24" s="9"/>
       <c r="L24" s="9">
@@ -2179,32 +2160,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="7" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>125</v>
+        <v>43</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>126</v>
+        <v>45</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>127</v>
+        <v>46</v>
       </c>
       <c r="J25" s="8">
         <v>1</v>
@@ -2215,211 +2195,208 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>45</v>
+      <c r="B26" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" s="52">
+        <v>0</v>
+      </c>
+      <c r="D26" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="48" t="s">
+        <v>149</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="J26" s="8">
-        <v>1</v>
-      </c>
-      <c r="K26" s="9"/>
+        <v>150</v>
+      </c>
+      <c r="J26" s="48">
+        <v>5</v>
+      </c>
+      <c r="K26" s="48"/>
       <c r="L26" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M26" s="48"/>
+    </row>
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B27" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C27" s="53">
-        <v>0</v>
-      </c>
-      <c r="D27" s="50" t="s">
+      <c r="B27" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="49" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="49" t="s">
-        <v>148</v>
+      <c r="F27" s="14" t="s">
+        <v>151</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="49" t="s">
-        <v>149</v>
+      <c r="H27" s="14" t="s">
+        <v>152</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="J27" s="49">
-        <v>5</v>
-      </c>
-      <c r="K27" s="49"/>
+        <v>153</v>
+      </c>
+      <c r="J27" s="50">
+        <v>4</v>
+      </c>
+      <c r="K27" s="51"/>
       <c r="L27" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M27" s="49"/>
+      <c r="M27" s="48"/>
     </row>
     <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D28" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" s="49" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G28" s="14" t="s">
         <v>11</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="J28" s="51">
+        <v>156</v>
+      </c>
+      <c r="J28" s="50">
         <v>4</v>
       </c>
-      <c r="K28" s="52"/>
+      <c r="K28" s="51"/>
       <c r="L28" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M28" s="49"/>
+      <c r="M28" s="48"/>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="D29" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="14" t="s">
-        <v>19</v>
+      <c r="E29" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="G29" s="14" t="s">
         <v>11</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="J29" s="51">
+        <v>159</v>
+      </c>
+      <c r="J29" s="50">
         <v>4</v>
       </c>
-      <c r="K29" s="52"/>
+      <c r="K29" s="51"/>
       <c r="L29" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M29" s="49"/>
+      <c r="M29" s="48"/>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>15</v>
+        <v>171</v>
+      </c>
+      <c r="C30" s="14">
+        <v>0</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="G30" s="14" t="s">
         <v>11</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="J30" s="51">
-        <v>4</v>
-      </c>
-      <c r="K30" s="52"/>
+        <v>176</v>
+      </c>
+      <c r="J30" s="50">
+        <v>3</v>
+      </c>
+      <c r="K30" s="51"/>
       <c r="L30" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M30" s="49"/>
+      <c r="M30" s="48"/>
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C31" s="14">
-        <v>0</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>175</v>
+        <v>142</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D31" s="49" t="s">
+        <v>14</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>19</v>
@@ -2431,223 +2408,209 @@
         <v>11</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="J31" s="51">
-        <v>3</v>
-      </c>
-      <c r="K31" s="52"/>
+        <v>179</v>
+      </c>
+      <c r="J31" s="50">
+        <v>1</v>
+      </c>
+      <c r="K31" s="51"/>
       <c r="L31" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="49"/>
-    </row>
-    <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <f>J31*K31</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="48"/>
+    </row>
+    <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="D32" s="50" t="s">
+      <c r="B32" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="G32" s="14" t="s">
+      <c r="E32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32" t="s">
+        <v>84</v>
+      </c>
+      <c r="G32" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" t="s">
+        <v>85</v>
+      </c>
+      <c r="I32" t="s">
+        <v>86</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="L32"/>
+    </row>
+    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>30</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" t="s">
+        <v>181</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" t="s">
+        <v>160</v>
+      </c>
+      <c r="G33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H33" t="s">
+        <v>161</v>
+      </c>
+      <c r="I33" t="s">
+        <v>162</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="L33"/>
+    </row>
+    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>31</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C34" t="s">
+        <v>182</v>
+      </c>
+      <c r="D34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" t="s">
+        <v>44</v>
+      </c>
+      <c r="H34" t="s">
+        <v>164</v>
+      </c>
+      <c r="I34" t="s">
+        <v>165</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="L34"/>
+    </row>
+    <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>32</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35" t="s">
+        <v>166</v>
+      </c>
+      <c r="F35" t="s">
+        <v>168</v>
+      </c>
+      <c r="G35" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="J32" s="51">
+      <c r="H35" t="s">
+        <v>167</v>
+      </c>
+      <c r="I35" t="s">
+        <v>169</v>
+      </c>
+      <c r="J35">
         <v>1</v>
       </c>
-      <c r="K32" s="52"/>
-      <c r="L32" s="9">
-        <f>J32*K32</f>
-        <v>0</v>
-      </c>
-      <c r="M32" s="49"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="46">
-        <f>A32+1</f>
-        <v>30</v>
-      </c>
-      <c r="B33" s="43" t="s">
+      <c r="L35"/>
+    </row>
+    <row r="36" spans="1:12" s="58" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="61">
+        <v>33</v>
+      </c>
+      <c r="B36" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="D36" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="G36" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="H36" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="I36" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="J36" s="56">
+        <v>1</v>
+      </c>
+      <c r="K36" s="57"/>
+      <c r="L36" s="57">
+        <f>J36*K36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="61">
+        <v>34</v>
+      </c>
+      <c r="B37" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C37" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="45">
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="45">
         <v>7</v>
       </c>
-      <c r="K33" s="47"/>
-      <c r="L33" s="9"/>
-    </row>
-    <row r="34" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="46">
-        <f t="shared" ref="A34:A37" si="2">A33+1</f>
-        <v>31</v>
-      </c>
-      <c r="B34" s="54" t="s">
-        <v>144</v>
-      </c>
-      <c r="C34" s="55" t="s">
-        <v>170</v>
-      </c>
-      <c r="D34" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="G34" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="H34" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="I34" s="54" t="s">
-        <v>86</v>
-      </c>
-      <c r="J34" s="57">
-        <v>1</v>
-      </c>
-      <c r="K34" s="58"/>
-      <c r="L34" s="9"/>
-    </row>
-    <row r="35" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="46">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="B35" s="54" t="s">
-        <v>137</v>
-      </c>
-      <c r="C35" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="D35" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="G35" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="H35" s="55" t="s">
-        <v>161</v>
-      </c>
-      <c r="I35" s="54" t="s">
-        <v>162</v>
-      </c>
-      <c r="J35" s="57">
-        <v>1</v>
-      </c>
-      <c r="K35" s="58"/>
-      <c r="L35" s="9"/>
-    </row>
-    <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="46">
-        <f t="shared" si="2"/>
-        <v>33</v>
-      </c>
-      <c r="B36" s="54" t="s">
-        <v>143</v>
-      </c>
-      <c r="C36" s="55" t="s">
-        <v>172</v>
-      </c>
-      <c r="D36" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" s="54" t="s">
-        <v>163</v>
-      </c>
-      <c r="G36" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="H36" s="55" t="s">
-        <v>164</v>
-      </c>
-      <c r="I36" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="J36" s="57">
-        <v>1</v>
-      </c>
-      <c r="K36" s="58"/>
-      <c r="L36" s="9"/>
-    </row>
-    <row r="37" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="46">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="B37" s="54" t="s">
-        <v>145</v>
-      </c>
-      <c r="C37" s="55" t="s">
-        <v>112</v>
-      </c>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55" t="s">
-        <v>166</v>
-      </c>
-      <c r="F37" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="G37" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="55" t="s">
-        <v>167</v>
-      </c>
-      <c r="I37" s="54" t="s">
-        <v>169</v>
-      </c>
-      <c r="J37" s="57">
-        <v>1</v>
-      </c>
-      <c r="K37" s="58"/>
+      <c r="K37" s="46"/>
       <c r="L37" s="9"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
@@ -2657,12 +2620,12 @@
       <c r="I38" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="J38" s="48">
+      <c r="J38" s="47">
         <f>SUM(J4:J37)</f>
         <v>111</v>
       </c>
       <c r="L38" s="3">
-        <f>SUM(L4:L27)</f>
+        <f>SUM(L4:L26)</f>
         <v>0</v>
       </c>
     </row>
@@ -2670,6 +2633,7 @@
       <c r="B39" s="17"/>
     </row>
     <row r="40" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="62"/>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>

</xml_diff>

<commit_message>
- RF board BOMs updated with switches
</commit_message>
<xml_diff>
--- a/hardware/RFWBBoard/RFWBBoard_BOM.xlsx
+++ b/hardware/RFWBBoard/RFWBBoard_BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="191">
   <si>
     <t>Item #</t>
   </si>
@@ -569,6 +569,30 @@
   </si>
   <si>
     <t>33pF</t>
+  </si>
+  <si>
+    <t>SWITCH-CJS-1200-1200</t>
+  </si>
+  <si>
+    <t>J-Lead</t>
+  </si>
+  <si>
+    <t>CJS</t>
+  </si>
+  <si>
+    <t>CJS-1200TA</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>563-1021-1-ND</t>
+  </si>
+  <si>
+    <t>CJS-1200 SPDT Switch</t>
+  </si>
+  <si>
+    <t>SW1, SW2, SW3, SW4</t>
   </si>
 </sst>
 </file>
@@ -578,12 +602,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -645,6 +676,21 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -757,14 +803,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -774,7 +821,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -789,13 +836,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -807,19 +854,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -839,48 +886,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -892,39 +930,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Excel_BuiltIn_Calculation 1" xfId="3"/>
     <cellStyle name="Excel_BuiltIn_Explanatory Text 1" xfId="2"/>
     <cellStyle name="Excel_BuiltIn_Heading 3 1" xfId="1"/>
+    <cellStyle name="Explanatory Text" xfId="5" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
@@ -1313,18 +1361,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="46.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="1" customWidth="1"/>
@@ -1337,20 +1385,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2" s="4"/>
@@ -1364,40 +1412,40 @@
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="41" t="s">
+      <c r="A3" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="41" t="s">
+      <c r="L3" s="38" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2202,36 +2250,36 @@
       <c r="B26" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="C26" s="52">
-        <v>0</v>
-      </c>
-      <c r="D26" s="49" t="s">
+      <c r="C26" s="49">
+        <v>0</v>
+      </c>
+      <c r="D26" s="46" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="48" t="s">
+      <c r="F26" s="45" t="s">
         <v>148</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="48" t="s">
+      <c r="H26" s="45" t="s">
         <v>149</v>
       </c>
       <c r="I26" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="J26" s="48">
+      <c r="J26" s="45">
         <v>5</v>
       </c>
-      <c r="K26" s="48"/>
+      <c r="K26" s="45"/>
       <c r="L26" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M26" s="48"/>
+      <c r="M26" s="45"/>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
@@ -2243,7 +2291,7 @@
       <c r="C27" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="49" t="s">
+      <c r="D27" s="46" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="14" t="s">
@@ -2261,15 +2309,15 @@
       <c r="I27" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="J27" s="50">
+      <c r="J27" s="47">
         <v>4</v>
       </c>
-      <c r="K27" s="51"/>
+      <c r="K27" s="48"/>
       <c r="L27" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M27" s="48"/>
+      <c r="M27" s="45"/>
     </row>
     <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
@@ -2281,7 +2329,7 @@
       <c r="C28" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D28" s="49" t="s">
+      <c r="D28" s="46" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="14" t="s">
@@ -2299,15 +2347,15 @@
       <c r="I28" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="J28" s="50">
+      <c r="J28" s="47">
         <v>4</v>
       </c>
-      <c r="K28" s="51"/>
+      <c r="K28" s="48"/>
       <c r="L28" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M28" s="48"/>
+      <c r="M28" s="45"/>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
@@ -2319,7 +2367,7 @@
       <c r="C29" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="49" t="s">
+      <c r="D29" s="46" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="6" t="s">
@@ -2337,15 +2385,15 @@
       <c r="I29" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="J29" s="50">
+      <c r="J29" s="47">
         <v>4</v>
       </c>
-      <c r="K29" s="51"/>
+      <c r="K29" s="48"/>
       <c r="L29" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M29" s="48"/>
+      <c r="M29" s="45"/>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
@@ -2375,15 +2423,15 @@
       <c r="I30" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="J30" s="50">
+      <c r="J30" s="47">
         <v>3</v>
       </c>
-      <c r="K30" s="51"/>
+      <c r="K30" s="48"/>
       <c r="L30" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M30" s="48"/>
+      <c r="M30" s="45"/>
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
@@ -2395,7 +2443,7 @@
       <c r="C31" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="D31" s="49" t="s">
+      <c r="D31" s="46" t="s">
         <v>14</v>
       </c>
       <c r="E31" s="14" t="s">
@@ -2413,15 +2461,15 @@
       <c r="I31" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="J31" s="50">
+      <c r="J31" s="47">
         <v>1</v>
       </c>
-      <c r="K31" s="51"/>
+      <c r="K31" s="48"/>
       <c r="L31" s="9">
         <f>J31*K31</f>
         <v>0</v>
       </c>
-      <c r="M31" s="48"/>
+      <c r="M31" s="45"/>
     </row>
     <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
@@ -2454,7 +2502,10 @@
       <c r="J32">
         <v>1</v>
       </c>
-      <c r="L32"/>
+      <c r="L32" s="9">
+        <f t="shared" ref="L32:L36" si="1">J32*K32</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
@@ -2487,7 +2538,10 @@
       <c r="J33">
         <v>1</v>
       </c>
-      <c r="L33"/>
+      <c r="L33" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
@@ -2520,7 +2574,10 @@
       <c r="J34">
         <v>1</v>
       </c>
-      <c r="L34"/>
+      <c r="L34" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
@@ -2549,150 +2606,174 @@
       <c r="J35">
         <v>1</v>
       </c>
-      <c r="L35"/>
-    </row>
-    <row r="36" spans="1:12" s="58" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="61">
+      <c r="L35" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
         <v>33</v>
       </c>
-      <c r="B36" s="53" t="s">
+      <c r="B36" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="C36" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="D36" s="62" t="s">
+        <v>184</v>
+      </c>
+      <c r="E36" s="62" t="s">
+        <v>185</v>
+      </c>
+      <c r="F36" s="62" t="s">
+        <v>186</v>
+      </c>
+      <c r="G36" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="H36" s="62" t="s">
+        <v>188</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J36" s="44">
+        <v>4</v>
+      </c>
+      <c r="L36" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="55" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="56">
+        <v>34</v>
+      </c>
+      <c r="B37" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="C36" s="54" t="s">
+      <c r="C37" s="51" t="s">
         <v>170</v>
       </c>
-      <c r="D36" s="55" t="s">
+      <c r="D37" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="E36" s="54" t="s">
+      <c r="E37" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="54" t="s">
+      <c r="F37" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="G36" s="54" t="s">
+      <c r="G37" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="H36" s="54" t="s">
+      <c r="H37" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="I36" s="53" t="s">
+      <c r="I37" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="J36" s="56">
+      <c r="J37" s="53">
         <v>1</v>
       </c>
-      <c r="K36" s="57"/>
-      <c r="L36" s="57">
-        <f>J36*K36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="61">
-        <v>34</v>
-      </c>
-      <c r="B37" s="43" t="s">
+      <c r="K37" s="54"/>
+      <c r="L37" s="54"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="56">
+        <v>35</v>
+      </c>
+      <c r="B38" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="C37" s="44" t="s">
+      <c r="C38" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="45">
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="42">
         <v>7</v>
       </c>
-      <c r="K37" s="46"/>
-      <c r="L37" s="9"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="42" t="s">
+      <c r="K38" s="43"/>
+      <c r="L38" s="64"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="J38" s="47">
-        <f>SUM(J4:J37)</f>
-        <v>111</v>
-      </c>
-      <c r="L38" s="3">
+      <c r="J39" s="44">
+        <f>SUM(J4:J38)</f>
+        <v>115</v>
+      </c>
+      <c r="L39" s="3">
         <f>SUM(L4:L26)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B39" s="17"/>
-    </row>
-    <row r="40" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="62"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="18"/>
-      <c r="L40" s="3"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="20"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="23"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="17"/>
+    </row>
+    <row r="41" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="57"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="18"/>
+      <c r="L41" s="3"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="17"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="23"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
-      <c r="J43"/>
-      <c r="L43"/>
+      <c r="B43" s="17"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="27"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
       <c r="J44"/>
       <c r="L44"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="31"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="27"/>
       <c r="J45"/>
       <c r="L45"/>
     </row>
@@ -2709,34 +2790,38 @@
       <c r="L46"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="31"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="4"/>
+      <c r="L47" s="61"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="37"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="4"/>
+      <c r="L48"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="30"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="28"/>
-      <c r="I49" s="38"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="34"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="30"/>
@@ -2746,17 +2831,27 @@
       <c r="F50" s="28"/>
       <c r="G50" s="28"/>
       <c r="H50" s="28"/>
-      <c r="I50" s="38"/>
+      <c r="I50" s="35"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="39"/>
-      <c r="C51" s="40"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="28"/>
       <c r="D51" s="28"/>
       <c r="E51" s="28"/>
       <c r="F51" s="28"/>
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
-      <c r="I51" s="38"/>
+      <c r="I51" s="35"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="36"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="35"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>